<commit_message>
COst clutch actuation system
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/FR/FR_A0600/FRA0600.xlsx
+++ b/CR - Cost Report/BOM/FR/FR_A0600/FRA0600.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>System</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>FR_A0600</t>
+  </si>
+  <si>
+    <t>Bronze rings</t>
+  </si>
+  <si>
+    <t>Lubrificating rings for the lever</t>
+  </si>
+  <si>
+    <t>FR_06006</t>
   </si>
 </sst>
 </file>
@@ -516,7 +525,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,9 +535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -673,11 +682,21 @@
     <row r="8" spans="1:7" ht="15.75" thickBot="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>